<commit_message>
IndMF- Added color for NAV
</commit_message>
<xml_diff>
--- a/Reports/IndMFData/IndMF.xlsx
+++ b/Reports/IndMFData/IndMF.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/i852841/_Codes/_Personal/StockRankingCrawler/Reports/IndMFData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D073E050-4FD4-CD44-A299-BA264FB62BB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EC0A529-5613-1844-8936-4A86A0FFA154}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18880" yWindow="1400" windowWidth="33600" windowHeight="19380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SmallCap" sheetId="1" r:id="rId1"/>
+    <sheet name="MultiCap" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
   <si>
     <t>Nov_21</t>
   </si>
@@ -95,6 +96,15 @@
   </si>
   <si>
     <t>Nov_20</t>
+  </si>
+  <si>
+    <t>MIRAE</t>
+  </si>
+  <si>
+    <t>PARAGPARIKH</t>
+  </si>
+  <si>
+    <t>Nov_22</t>
   </si>
 </sst>
 </file>
@@ -110,12 +120,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="45"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="45"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -130,10 +155,54 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,9 +517,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -458,300 +527,638 @@
   <cols>
     <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="7.6640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.1640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>24</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="3">
+        <v>41.023000000000003</v>
+      </c>
+      <c r="C2" s="1">
         <v>41.113</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>41.27</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>41.249000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="4">
+        <v>23.527000000000001</v>
+      </c>
+      <c r="C3" s="1">
         <v>23.579000000000001</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>23.652000000000001</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>23.59</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="5">
+        <v>33.54</v>
+      </c>
+      <c r="C4" s="1">
         <v>33.71</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>33.770000000000003</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>33.83</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="6">
+        <v>58.055500000000002</v>
+      </c>
+      <c r="C5" s="1">
         <v>58.023200000000003</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>57.835700000000003</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>57.826599999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="7">
+        <v>77.438999999999993</v>
+      </c>
+      <c r="C6" s="1">
         <v>77.471000000000004</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>77.86</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>77.799000000000007</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="8">
+        <v>40.747599999999998</v>
+      </c>
+      <c r="C7" s="1">
         <v>40.936599999999999</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>40.968499999999999</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>40.872599999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="9">
+        <v>54.134</v>
+      </c>
+      <c r="C8" s="1">
         <v>54.107999999999997</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>54.265000000000001</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>54.210999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="10">
+        <v>26.14</v>
+      </c>
+      <c r="C9" s="1">
         <v>26.13</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>26.13</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>26.14</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="11">
+        <v>10.748900000000001</v>
+      </c>
+      <c r="C10" s="1">
         <v>10.723800000000001</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>10.7376</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>10.7271</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="12">
+        <v>32.220500000000001</v>
+      </c>
+      <c r="C11" s="1">
         <v>32.224699999999999</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>32.270899999999997</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>32.126399999999997</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="13">
+        <v>10.5183</v>
+      </c>
+      <c r="C12" s="1">
         <v>10.5168</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>10.5443</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="14">
+        <v>9.42</v>
+      </c>
+      <c r="C13" s="1">
         <v>9.4600000000000009</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>9.51</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="15">
+        <v>78.046800000000005</v>
+      </c>
+      <c r="C14" s="1">
         <v>78.256200000000007</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>78.58</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="16">
+        <v>10.75</v>
+      </c>
+      <c r="C15" s="1">
         <v>10.76</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>10.79</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>10.83</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="17">
+        <v>10.945</v>
+      </c>
+      <c r="C16" s="1">
         <v>10.984</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>10.988</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>10.986000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="18">
+        <v>52.753599999999999</v>
+      </c>
+      <c r="C17" s="1">
         <v>52.781399999999998</v>
       </c>
-      <c r="C17">
+      <c r="D17">
         <v>52.896900000000002</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>52.9773</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="19">
+        <v>10.38</v>
+      </c>
+      <c r="C18" s="1">
         <v>10.45</v>
       </c>
-      <c r="C18">
+      <c r="D18">
         <v>10.49</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="20">
+        <v>9.5</v>
+      </c>
+      <c r="C19" s="1">
         <v>9.5399999999999991</v>
       </c>
-      <c r="C19">
+      <c r="D19">
         <v>9.56</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="21">
+        <v>45.351399999999998</v>
+      </c>
+      <c r="C20" s="1">
         <v>45.565100000000001</v>
       </c>
-      <c r="C20">
+      <c r="D20">
         <v>45.5505</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="22">
+        <v>10.25</v>
+      </c>
+      <c r="C21" s="1">
         <v>10.27</v>
       </c>
-      <c r="C21">
+      <c r="D21">
         <v>10.25</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="23">
+        <v>41.302799999999998</v>
+      </c>
+      <c r="C22" s="1">
         <v>41.552900000000001</v>
       </c>
-      <c r="C22">
+      <c r="D22">
         <v>41.19</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="24">
+        <v>14.44</v>
+      </c>
+      <c r="C23" s="1">
         <v>14.49</v>
       </c>
-      <c r="C23">
+      <c r="D23">
         <v>14.51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="25">
+        <v>82.435000000000002</v>
+      </c>
+      <c r="C2" s="1">
+        <v>82.471999999999994</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="26">
+        <v>11.48</v>
+      </c>
+      <c r="C3" s="1">
+        <v>11.574</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="27">
+        <v>32.76</v>
+      </c>
+      <c r="C4" s="1">
+        <v>32.89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="28">
+        <v>160.44880000000001</v>
+      </c>
+      <c r="C5" s="1">
+        <v>161.5027</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="29">
+        <v>39.33</v>
+      </c>
+      <c r="C6" s="1">
+        <v>39.587000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="30">
+        <v>101.17919999999999</v>
+      </c>
+      <c r="C7" s="1">
+        <v>101.31010000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="31">
+        <v>43.768999999999998</v>
+      </c>
+      <c r="C8" s="1">
+        <v>44.024999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="32">
+        <v>310.5</v>
+      </c>
+      <c r="C9" s="1">
+        <v>310.79000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="33">
+        <v>34.232900000000001</v>
+      </c>
+      <c r="C10" s="1">
+        <v>34.395899999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="34">
+        <v>796.42</v>
+      </c>
+      <c r="C11" s="1">
+        <v>799.82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="35">
+        <v>28.164899999999999</v>
+      </c>
+      <c r="C12" s="1">
+        <v>28.381699999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="36">
+        <v>23.4</v>
+      </c>
+      <c r="C13" s="1">
+        <v>23.54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="37">
+        <v>10.701000000000001</v>
+      </c>
+      <c r="C14" s="1">
+        <v>10.7348</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="38">
+        <v>52.4</v>
+      </c>
+      <c r="C15" s="1">
+        <v>52.63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="39">
+        <v>15.545999999999999</v>
+      </c>
+      <c r="C16" s="1">
+        <v>15.647</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="40">
+        <v>44.926499999999997</v>
+      </c>
+      <c r="C17" s="1">
+        <v>45.029800000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="41">
+        <v>144.63999999999999</v>
+      </c>
+      <c r="C18" s="1">
+        <v>145.69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="42">
+        <v>148.35</v>
+      </c>
+      <c r="C19" s="1">
+        <v>148.87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="43">
+        <v>194.56909999999999</v>
+      </c>
+      <c r="C20" s="1">
+        <v>196.26480000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="44">
+        <v>21.42</v>
+      </c>
+      <c r="C21" s="1">
+        <v>21.55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="45">
+        <v>11.754</v>
+      </c>
+      <c r="C22" s="1">
+        <v>11.81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="46">
+        <v>27.3172</v>
+      </c>
+      <c r="C23" s="1">
+        <v>27.501000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
IndMF- Added other attributes like pe,pb etc
</commit_message>
<xml_diff>
--- a/Reports/IndMFData/IndMF.xlsx
+++ b/Reports/IndMFData/IndMF.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/i852841/_Codes/_Personal/StockRankingCrawler/Reports/IndMFData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EC0A529-5613-1844-8936-4A86A0FFA154}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{5EC0A529-5613-1844-8936-4A86A0FFA154}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="1" windowHeight="19380" windowWidth="33600" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="460"/>
   </bookViews>
   <sheets>
-    <sheet name="SmallCap" sheetId="1" r:id="rId1"/>
-    <sheet name="MultiCap" sheetId="2" r:id="rId2"/>
+    <sheet name="SmallCap" r:id="rId1" sheetId="1"/>
+    <sheet name="MultiCap" r:id="rId2" sheetId="2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="30">
   <si>
     <t>Nov_21</t>
   </si>
@@ -105,12 +105,19 @@
   </si>
   <si>
     <t>Nov_22</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Nov_24</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -153,62 +160,84 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+  <cellXfs count="69">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="2" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -225,10 +254,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -263,7 +292,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -315,7 +344,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -426,21 +455,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -457,7 +486,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -509,14 +538,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -525,24 +554,28 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="7.6640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.1640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.83203125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="7.6640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="7.6640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.6640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="8.1640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="8.1640625" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="0" t="s">
         <v>23</v>
       </c>
     </row>
@@ -550,33 +583,39 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
-        <v>41.023000000000003</v>
-      </c>
-      <c r="C2" s="1">
+      <c r="B2" s="47" t="n">
+        <v>41.023</v>
+      </c>
+      <c r="C2" s="3" t="n">
+        <v>41.023</v>
+      </c>
+      <c r="D2" s="1" t="n">
         <v>41.113</v>
       </c>
-      <c r="D2">
+      <c r="E2" s="0" t="n">
         <v>41.27</v>
       </c>
-      <c r="E2">
-        <v>41.249000000000002</v>
+      <c r="F2" s="0" t="n">
+        <v>41.249</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4">
-        <v>23.527000000000001</v>
-      </c>
-      <c r="C3" s="1">
-        <v>23.579000000000001</v>
-      </c>
-      <c r="D3">
-        <v>23.652000000000001</v>
-      </c>
-      <c r="E3">
+      <c r="B3" s="48" t="n">
+        <v>23.527</v>
+      </c>
+      <c r="C3" s="4" t="n">
+        <v>23.527</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>23.579</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>23.652</v>
+      </c>
+      <c r="F3" s="0" t="n">
         <v>23.59</v>
       </c>
     </row>
@@ -584,16 +623,19 @@
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="49" t="n">
         <v>33.54</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="5" t="n">
+        <v>33.54</v>
+      </c>
+      <c r="D4" s="1" t="n">
         <v>33.71</v>
       </c>
-      <c r="D4">
-        <v>33.770000000000003</v>
-      </c>
-      <c r="E4">
+      <c r="E4" s="0" t="n">
+        <v>33.77</v>
+      </c>
+      <c r="F4" s="0" t="n">
         <v>33.83</v>
       </c>
     </row>
@@ -601,84 +643,99 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="6">
-        <v>58.055500000000002</v>
-      </c>
-      <c r="C5" s="1">
-        <v>58.023200000000003</v>
-      </c>
-      <c r="D5">
-        <v>57.835700000000003</v>
-      </c>
-      <c r="E5">
-        <v>57.826599999999999</v>
+      <c r="B5" s="50" t="n">
+        <v>58.0555</v>
+      </c>
+      <c r="C5" s="6" t="n">
+        <v>58.0555</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>58.0232</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>57.8357</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>57.8266</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="7">
-        <v>77.438999999999993</v>
-      </c>
-      <c r="C6" s="1">
-        <v>77.471000000000004</v>
-      </c>
-      <c r="D6">
+      <c r="B6" s="51" t="n">
+        <v>77.439</v>
+      </c>
+      <c r="C6" s="7" t="n">
+        <v>77.439</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>77.471</v>
+      </c>
+      <c r="E6" s="0" t="n">
         <v>77.86</v>
       </c>
-      <c r="E6">
-        <v>77.799000000000007</v>
+      <c r="F6" s="0" t="n">
+        <v>77.799</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="8">
-        <v>40.747599999999998</v>
-      </c>
-      <c r="C7" s="1">
-        <v>40.936599999999999</v>
-      </c>
-      <c r="D7">
-        <v>40.968499999999999</v>
-      </c>
-      <c r="E7">
-        <v>40.872599999999998</v>
+      <c r="B7" s="52" t="n">
+        <v>40.7476</v>
+      </c>
+      <c r="C7" s="8" t="n">
+        <v>40.7476</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>40.9366</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>40.9685</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>40.8726</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="53" t="n">
         <v>54.134</v>
       </c>
-      <c r="C8" s="1">
-        <v>54.107999999999997</v>
-      </c>
-      <c r="D8">
-        <v>54.265000000000001</v>
-      </c>
-      <c r="E8">
-        <v>54.210999999999999</v>
+      <c r="C8" s="9" t="n">
+        <v>54.134</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>54.108</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>54.265</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>54.211</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="54" t="n">
         <v>26.14</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="10" t="n">
+        <v>26.14</v>
+      </c>
+      <c r="D9" s="1" t="n">
         <v>26.13</v>
       </c>
-      <c r="D9">
+      <c r="E9" s="0" t="n">
         <v>26.13</v>
       </c>
-      <c r="E9">
+      <c r="F9" s="0" t="n">
         <v>26.14</v>
       </c>
     </row>
@@ -686,16 +743,19 @@
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="11">
-        <v>10.748900000000001</v>
-      </c>
-      <c r="C10" s="1">
-        <v>10.723800000000001</v>
-      </c>
-      <c r="D10">
+      <c r="B10" s="55" t="n">
+        <v>10.7489</v>
+      </c>
+      <c r="C10" s="11" t="n">
+        <v>10.7489</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>10.7238</v>
+      </c>
+      <c r="E10" s="0" t="n">
         <v>10.7376</v>
       </c>
-      <c r="E10">
+      <c r="F10" s="0" t="n">
         <v>10.7271</v>
       </c>
     </row>
@@ -703,30 +763,36 @@
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="12">
-        <v>32.220500000000001</v>
-      </c>
-      <c r="C11" s="1">
-        <v>32.224699999999999</v>
-      </c>
-      <c r="D11">
-        <v>32.270899999999997</v>
-      </c>
-      <c r="E11">
-        <v>32.126399999999997</v>
+      <c r="B11" s="56" t="n">
+        <v>32.2205</v>
+      </c>
+      <c r="C11" s="12" t="n">
+        <v>32.2205</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>32.2247</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>32.2709</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>32.1264</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="13">
+      <c r="B12" s="57" t="n">
         <v>10.5183</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="13" t="n">
+        <v>10.5183</v>
+      </c>
+      <c r="D12" s="1" t="n">
         <v>10.5168</v>
       </c>
-      <c r="D12">
+      <c r="E12" s="0" t="n">
         <v>10.5443</v>
       </c>
     </row>
@@ -734,13 +800,16 @@
       <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="14">
+      <c r="B13" s="58" t="n">
         <v>9.42</v>
       </c>
-      <c r="C13" s="1">
-        <v>9.4600000000000009</v>
-      </c>
-      <c r="D13">
+      <c r="C13" s="14" t="n">
+        <v>9.42</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>9.46</v>
+      </c>
+      <c r="E13" s="0" t="n">
         <v>9.51</v>
       </c>
     </row>
@@ -748,13 +817,16 @@
       <c r="A14" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="15">
-        <v>78.046800000000005</v>
-      </c>
-      <c r="C14" s="1">
-        <v>78.256200000000007</v>
-      </c>
-      <c r="D14">
+      <c r="B14" s="59" t="n">
+        <v>78.0468</v>
+      </c>
+      <c r="C14" s="15" t="n">
+        <v>78.0468</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>78.2562</v>
+      </c>
+      <c r="E14" s="0" t="n">
         <v>78.58</v>
       </c>
     </row>
@@ -762,16 +834,19 @@
       <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="16">
+      <c r="B15" s="60" t="n">
         <v>10.75</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="16" t="n">
+        <v>10.75</v>
+      </c>
+      <c r="D15" s="1" t="n">
         <v>10.76</v>
       </c>
-      <c r="D15">
+      <c r="E15" s="0" t="n">
         <v>10.79</v>
       </c>
-      <c r="E15">
+      <c r="F15" s="0" t="n">
         <v>10.83</v>
       </c>
     </row>
@@ -779,33 +854,39 @@
       <c r="A16" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="17">
+      <c r="B16" s="61" t="n">
         <v>10.945</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="17" t="n">
+        <v>10.945</v>
+      </c>
+      <c r="D16" s="1" t="n">
         <v>10.984</v>
       </c>
-      <c r="D16">
+      <c r="E16" s="0" t="n">
         <v>10.988</v>
       </c>
-      <c r="E16">
-        <v>10.986000000000001</v>
+      <c r="F16" s="0" t="n">
+        <v>10.986</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="18">
-        <v>52.753599999999999</v>
-      </c>
-      <c r="C17" s="1">
-        <v>52.781399999999998</v>
-      </c>
-      <c r="D17">
-        <v>52.896900000000002</v>
-      </c>
-      <c r="E17">
+      <c r="B17" s="62" t="n">
+        <v>52.7536</v>
+      </c>
+      <c r="C17" s="18" t="n">
+        <v>52.7536</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>52.7814</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>52.8969</v>
+      </c>
+      <c r="F17" s="0" t="n">
         <v>52.9773</v>
       </c>
     </row>
@@ -813,13 +894,16 @@
       <c r="A18" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="19">
+      <c r="B18" s="63" t="n">
         <v>10.38</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="19" t="n">
+        <v>10.38</v>
+      </c>
+      <c r="D18" s="1" t="n">
         <v>10.45</v>
       </c>
-      <c r="D18">
+      <c r="E18" s="0" t="n">
         <v>10.49</v>
       </c>
     </row>
@@ -827,13 +911,16 @@
       <c r="A19" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="20">
+      <c r="B19" s="64" t="n">
         <v>9.5</v>
       </c>
-      <c r="C19" s="1">
-        <v>9.5399999999999991</v>
-      </c>
-      <c r="D19">
+      <c r="C19" s="20" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>9.54</v>
+      </c>
+      <c r="E19" s="0" t="n">
         <v>9.56</v>
       </c>
     </row>
@@ -841,13 +928,16 @@
       <c r="A20" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="21">
-        <v>45.351399999999998</v>
-      </c>
-      <c r="C20" s="1">
-        <v>45.565100000000001</v>
-      </c>
-      <c r="D20">
+      <c r="B20" s="65" t="n">
+        <v>45.3514</v>
+      </c>
+      <c r="C20" s="21" t="n">
+        <v>45.3514</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <v>45.5651</v>
+      </c>
+      <c r="E20" s="0" t="n">
         <v>45.5505</v>
       </c>
     </row>
@@ -855,13 +945,16 @@
       <c r="A21" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="22">
+      <c r="B21" s="66" t="n">
         <v>10.25</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="22" t="n">
+        <v>10.25</v>
+      </c>
+      <c r="D21" s="1" t="n">
         <v>10.27</v>
       </c>
-      <c r="D21">
+      <c r="E21" s="0" t="n">
         <v>10.25</v>
       </c>
     </row>
@@ -869,13 +962,16 @@
       <c r="A22" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="23">
-        <v>41.302799999999998</v>
-      </c>
-      <c r="C22" s="1">
-        <v>41.552900000000001</v>
-      </c>
-      <c r="D22">
+      <c r="B22" s="67" t="n">
+        <v>41.3028</v>
+      </c>
+      <c r="C22" s="23" t="n">
+        <v>41.3028</v>
+      </c>
+      <c r="D22" s="1" t="n">
+        <v>41.5529</v>
+      </c>
+      <c r="E22" s="0" t="n">
         <v>41.19</v>
       </c>
     </row>
@@ -883,23 +979,26 @@
       <c r="A23" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="24">
+      <c r="B23" s="68" t="n">
         <v>14.44</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" s="24" t="n">
+        <v>14.44</v>
+      </c>
+      <c r="D23" s="1" t="n">
         <v>14.49</v>
       </c>
-      <c r="D23">
+      <c r="E23" s="0" t="n">
         <v>14.51</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -908,7 +1007,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="8" customWidth="1"/>
+    <col min="3" max="3" customWidth="true" width="8.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -1162,6 +1261,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>